<commit_message>
Reportando los hallazgos de Massaro y Anderson
</commit_message>
<xml_diff>
--- a/Finanzas/Febrero_2017.xlsx
+++ b/Finanzas/Febrero_2017.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adriana\Desktop\Tesis_AdrianaFelCha\Finanzas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\Desktop\Felisa\Finanzas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="121">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -373,6 +373,21 @@
   <si>
     <t>='</t>
   </si>
+  <si>
+    <t>Mar</t>
+  </si>
+  <si>
+    <t>Yogurth; Copias</t>
+  </si>
+  <si>
+    <t>Ver a Pedro en la Vasconcelos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOMINGO :D :D :D </t>
+  </si>
+  <si>
+    <t>Mamá coopero para mi yogurth :D</t>
+  </si>
 </sst>
 </file>
 
@@ -662,7 +677,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -782,6 +797,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1078,8 +1094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AZ598"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="S16" sqref="S16"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="U22" sqref="U22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1099,6 +1115,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A1" s="40"/>
       <c r="B1" s="55" t="s">
         <v>80</v>
       </c>
@@ -1382,7 +1399,7 @@
       </c>
       <c r="N4" s="5">
         <f>SUM(L3,L9)</f>
-        <v>27855.86</v>
+        <v>27995.86</v>
       </c>
       <c r="S4" s="49">
         <v>42783</v>
@@ -1477,7 +1494,7 @@
       </c>
       <c r="AY4" s="64">
         <f>(SUM((AO3:AO520)))-(SUM((AR3:AR520)))</f>
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="AZ4" s="64"/>
     </row>
@@ -1596,6 +1613,7 @@
       <c r="AZ5" s="64"/>
     </row>
     <row r="6" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A6" s="40"/>
       <c r="I6" s="32"/>
       <c r="J6" s="32"/>
       <c r="K6" s="54" t="s">
@@ -1603,7 +1621,7 @@
       </c>
       <c r="L6" s="54">
         <f>(SUM((Q11:Q500),(V3:V520)))-(SUM(E11:E500))</f>
-        <v>630.5</v>
+        <v>692.5</v>
       </c>
       <c r="M6" s="32"/>
       <c r="N6" s="32"/>
@@ -1634,6 +1652,9 @@
       <c r="AA6">
         <v>0</v>
       </c>
+      <c r="AB6" s="40" t="s">
+        <v>119</v>
+      </c>
       <c r="AD6">
         <v>0</v>
       </c>
@@ -1691,7 +1712,7 @@
       <c r="AU6">
         <v>0</v>
       </c>
-      <c r="AW6" s="64"/>
+      <c r="AW6" s="79"/>
       <c r="AX6" s="64"/>
       <c r="AY6" s="64"/>
       <c r="AZ6" s="64"/>
@@ -1794,26 +1815,41 @@
     </row>
     <row r="8" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A8" s="40"/>
+      <c r="K8" s="40"/>
       <c r="S8" s="49">
         <v>42787</v>
       </c>
-      <c r="T8" s="50"/>
-      <c r="U8" s="51"/>
+      <c r="T8" s="50" t="s">
+        <v>116</v>
+      </c>
+      <c r="U8" s="51" t="s">
+        <v>118</v>
+      </c>
       <c r="V8" s="43">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="W8" s="52"/>
-      <c r="X8" s="76"/>
+        <v>62</v>
+      </c>
+      <c r="W8" s="52">
+        <v>75</v>
+      </c>
+      <c r="X8" s="76">
+        <v>9</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>120</v>
+      </c>
       <c r="Z8" s="53">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>22</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>117</v>
       </c>
       <c r="AD8">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AE8">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AF8">
         <v>0</v>
@@ -1841,15 +1877,30 @@
       </c>
       <c r="AN8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="AO8">
+        <v>0</v>
+      </c>
+      <c r="AP8">
+        <v>2</v>
+      </c>
+      <c r="AQ8">
+        <v>2</v>
       </c>
       <c r="AR8">
         <f t="shared" si="4"/>
+        <v>22</v>
+      </c>
+      <c r="AS8">
         <v>0</v>
       </c>
       <c r="AT8">
         <f t="shared" si="3"/>
         <v>0</v>
+      </c>
+      <c r="AU8">
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:52" x14ac:dyDescent="0.25">
@@ -1871,7 +1922,7 @@
       </c>
       <c r="L9" s="15">
         <f>SUM(L11:L500)</f>
-        <v>23684</v>
+        <v>23824</v>
       </c>
       <c r="N9" s="35" t="s">
         <v>56</v>
@@ -1936,6 +1987,7 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
+      <c r="AV9" s="40"/>
     </row>
     <row r="10" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -2444,7 +2496,7 @@
         <v>42794</v>
       </c>
       <c r="T15" s="50"/>
-      <c r="U15" s="51"/>
+      <c r="U15" s="74"/>
       <c r="V15" s="43">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2523,7 +2575,9 @@
       <c r="O16" s="59"/>
       <c r="P16" s="59"/>
       <c r="Q16" s="39"/>
-      <c r="S16" s="50"/>
+      <c r="S16" s="49">
+        <v>42795</v>
+      </c>
       <c r="T16" s="50"/>
       <c r="U16" s="51"/>
       <c r="V16" s="43">
@@ -2604,7 +2658,9 @@
       <c r="O17" s="59"/>
       <c r="P17" s="59"/>
       <c r="Q17" s="39"/>
-      <c r="S17" s="50"/>
+      <c r="S17" s="49">
+        <v>42796</v>
+      </c>
       <c r="T17" s="50"/>
       <c r="U17" s="51"/>
       <c r="V17" s="43">
@@ -2685,7 +2741,9 @@
       <c r="O18" s="59"/>
       <c r="P18" s="59"/>
       <c r="Q18" s="39"/>
-      <c r="S18" s="50"/>
+      <c r="S18" s="49">
+        <v>42797</v>
+      </c>
       <c r="T18" s="50"/>
       <c r="U18" s="51"/>
       <c r="V18" s="43">
@@ -2766,7 +2824,9 @@
       <c r="O19" s="59"/>
       <c r="P19" s="59"/>
       <c r="Q19" s="39"/>
-      <c r="S19" s="50"/>
+      <c r="S19" s="49">
+        <v>42798</v>
+      </c>
       <c r="T19" s="50"/>
       <c r="U19" s="51"/>
       <c r="V19" s="43">
@@ -2847,7 +2907,9 @@
       <c r="O20" s="59"/>
       <c r="P20" s="59"/>
       <c r="Q20" s="39"/>
-      <c r="S20" s="50"/>
+      <c r="S20" s="49">
+        <v>42799</v>
+      </c>
       <c r="T20" s="50"/>
       <c r="U20" s="51"/>
       <c r="V20" s="43">
@@ -2928,7 +2990,9 @@
       <c r="O21" s="59"/>
       <c r="P21" s="59"/>
       <c r="Q21" s="39"/>
-      <c r="S21" s="50"/>
+      <c r="S21" s="49">
+        <v>42800</v>
+      </c>
       <c r="T21" s="50"/>
       <c r="U21" s="51"/>
       <c r="V21" s="43">
@@ -3011,7 +3075,9 @@
       <c r="O22" s="59"/>
       <c r="P22" s="59"/>
       <c r="Q22" s="39"/>
-      <c r="S22" s="50"/>
+      <c r="S22" s="49">
+        <v>42801</v>
+      </c>
       <c r="T22" s="50"/>
       <c r="U22" s="51"/>
       <c r="V22" s="43">
@@ -3246,14 +3312,14 @@
         <v>52</v>
       </c>
       <c r="J25" s="24">
-        <v>560</v>
+        <v>700</v>
       </c>
       <c r="K25" s="23">
         <v>0</v>
       </c>
       <c r="L25" s="21">
         <f t="shared" si="5"/>
-        <v>560</v>
+        <v>700</v>
       </c>
       <c r="N25" s="59"/>
       <c r="O25" s="59"/>

</xml_diff>

<commit_message>
Construyendo estimulos del Experimento 1
</commit_message>
<xml_diff>
--- a/Finanzas/Febrero_2017.xlsx
+++ b/Finanzas/Febrero_2017.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="157">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -490,6 +490,24 @@
   <si>
     <t>Chocolate</t>
   </si>
+  <si>
+    <t>Netflix - Marzo</t>
+  </si>
+  <si>
+    <t>?????</t>
+  </si>
+  <si>
+    <t>Casa Javs Llaves</t>
+  </si>
+  <si>
+    <t>Mamá -</t>
+  </si>
+  <si>
+    <t>Uriel</t>
+  </si>
+  <si>
+    <t>Olvide mi dinero en el coche'</t>
+  </si>
 </sst>
 </file>
 
@@ -800,7 +818,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -930,6 +948,7 @@
     <xf numFmtId="3" fontId="17" fillId="21" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1227,7 +1246,7 @@
   <dimension ref="A1:AZ598"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1298,7 +1317,7 @@
       </c>
       <c r="D2" s="84">
         <f>L3-C2</f>
-        <v>-5087.0600000000004</v>
+        <v>-5274.2800000000007</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>2</v>
@@ -1422,7 +1441,7 @@
       </c>
       <c r="L3" s="27">
         <f>(SUM(C2,(E11:E500),(K11:K500)))-(SUM((D11:D500),(C11:C500)))</f>
-        <v>4614.9399999999996</v>
+        <v>4427.7199999999993</v>
       </c>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
@@ -1536,7 +1555,7 @@
       </c>
       <c r="N4" s="5">
         <f>SUM(L3,L9)</f>
-        <v>28433.94</v>
+        <v>28256.720000000001</v>
       </c>
       <c r="S4" s="49">
         <v>42783</v>
@@ -1631,7 +1650,7 @@
       </c>
       <c r="AY4" s="64">
         <f>(SUM((AO3:AO520)))-(SUM((AR3:AR520)))</f>
-        <v>9</v>
+        <v>46</v>
       </c>
       <c r="AZ4" s="64"/>
     </row>
@@ -1758,7 +1777,7 @@
       </c>
       <c r="L6" s="54">
         <f>(SUM((Q11:Q500),(V3:V520)))-(SUM(E11:E500))</f>
-        <v>88.5</v>
+        <v>73.5</v>
       </c>
       <c r="M6" s="32"/>
       <c r="N6" s="32"/>
@@ -2065,7 +2084,7 @@
       </c>
       <c r="L9" s="15">
         <f>SUM(L11:L500)</f>
-        <v>23819</v>
+        <v>23829</v>
       </c>
       <c r="N9" s="35" t="s">
         <v>56</v>
@@ -2824,20 +2843,40 @@
       <c r="S15" s="49">
         <v>42794</v>
       </c>
-      <c r="T15" s="50"/>
-      <c r="U15" s="74"/>
+      <c r="T15" s="50" t="s">
+        <v>116</v>
+      </c>
+      <c r="U15" s="74" t="s">
+        <v>153</v>
+      </c>
       <c r="V15" s="43">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="W15" s="52"/>
-      <c r="X15" s="52"/>
+        <v>-15</v>
+      </c>
+      <c r="W15" s="52">
+        <v>75</v>
+      </c>
+      <c r="X15" s="52">
+        <v>40</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>154</v>
+      </c>
       <c r="Z15" s="53">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>130</v>
+      </c>
+      <c r="AA15">
+        <v>60</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>98</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>150</v>
       </c>
       <c r="AD15">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AE15">
         <v>0</v>
@@ -2868,14 +2907,29 @@
       </c>
       <c r="AN15">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>60</v>
+      </c>
+      <c r="AO15">
+        <v>60</v>
+      </c>
+      <c r="AP15">
+        <v>3</v>
+      </c>
+      <c r="AQ15">
+        <v>1</v>
       </c>
       <c r="AR15">
         <f t="shared" si="4"/>
+        <v>23</v>
+      </c>
+      <c r="AS15">
         <v>0</v>
       </c>
       <c r="AT15">
         <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AU15">
         <v>0</v>
       </c>
     </row>
@@ -3244,8 +3298,16 @@
       </c>
     </row>
     <row r="20" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A20" s="34">
+        <v>42794</v>
+      </c>
+      <c r="B20" t="s">
+        <v>151</v>
+      </c>
       <c r="C20" s="13"/>
-      <c r="D20" s="12"/>
+      <c r="D20" s="12">
+        <v>170</v>
+      </c>
       <c r="E20" s="14"/>
       <c r="G20" s="59"/>
       <c r="H20" s="59" t="s">
@@ -3327,8 +3389,16 @@
       </c>
     </row>
     <row r="21" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A21" s="34">
+        <v>42794</v>
+      </c>
+      <c r="B21" t="s">
+        <v>152</v>
+      </c>
       <c r="C21" s="13"/>
-      <c r="D21" s="12"/>
+      <c r="D21" s="12">
+        <v>17.22</v>
+      </c>
       <c r="E21" s="14"/>
       <c r="G21" s="59"/>
       <c r="H21" s="59" t="s">
@@ -4005,14 +4075,22 @@
       <c r="C29" s="13"/>
       <c r="D29" s="12"/>
       <c r="E29" s="14"/>
-      <c r="G29" s="59"/>
-      <c r="H29" s="59"/>
-      <c r="I29" s="59"/>
-      <c r="J29" s="24"/>
+      <c r="G29" s="60">
+        <v>42794</v>
+      </c>
+      <c r="H29" s="59" t="s">
+        <v>155</v>
+      </c>
+      <c r="I29" s="85" t="s">
+        <v>156</v>
+      </c>
+      <c r="J29" s="24">
+        <v>10</v>
+      </c>
       <c r="K29" s="23"/>
       <c r="L29" s="21">
         <f t="shared" ref="L29:L32" si="6">J29-K29</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="N29" s="59"/>
       <c r="O29" s="59"/>

</xml_diff>

<commit_message>
Finanzas del lunes y presentación de Mike
</commit_message>
<xml_diff>
--- a/Finanzas/Febrero_2017.xlsx
+++ b/Finanzas/Febrero_2017.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\Desktop\Felisa\Finanzas\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7545"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="209">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -615,6 +610,54 @@
   </si>
   <si>
     <t>Maíz</t>
+  </si>
+  <si>
+    <t>ADRI FEST</t>
+  </si>
+  <si>
+    <t>Enana y papá cooperaron</t>
+  </si>
+  <si>
+    <t>Perro negro</t>
+  </si>
+  <si>
+    <t>Enigma Enana; Karaoke x2 +30 enana; Alambre noche; Coca enana; Karaoke Brandon</t>
+  </si>
+  <si>
+    <t>??????</t>
+  </si>
+  <si>
+    <t>Helados Nutrisa</t>
+  </si>
+  <si>
+    <t>Uber Fallido</t>
+  </si>
+  <si>
+    <t>Descanso</t>
+  </si>
+  <si>
+    <t>Papá Uber</t>
+  </si>
+  <si>
+    <t>Mike Herrera</t>
+  </si>
+  <si>
+    <t>Pastel Carlos</t>
+  </si>
+  <si>
+    <t>Niño</t>
+  </si>
+  <si>
+    <t>Pastel Carlos cooperacha</t>
+  </si>
+  <si>
+    <t>Cine Pedro Ale</t>
+  </si>
+  <si>
+    <t>Copias; Chocolate</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ,</t>
   </si>
 </sst>
 </file>
@@ -1354,7 +1397,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1364,8 +1407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BE964"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1395,6 +1438,7 @@
       <c r="D1" s="82" t="s">
         <v>147</v>
       </c>
+      <c r="P1" s="78"/>
       <c r="S1" s="46"/>
       <c r="T1" s="46"/>
       <c r="U1" s="46"/>
@@ -1438,7 +1482,7 @@
       </c>
       <c r="D2" s="86">
         <f>L3-C2</f>
-        <v>-4891.0200000000013</v>
+        <v>-5802.6900000000005</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>2</v>
@@ -1565,7 +1609,7 @@
       </c>
       <c r="L3" s="27">
         <f>(SUM(C2,(E11:E500),(K11:K500)))-(SUM((D11:D500),(C11:C500)))</f>
-        <v>4810.9799999999987</v>
+        <v>3899.3099999999995</v>
       </c>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
@@ -1682,7 +1726,7 @@
       </c>
       <c r="N4" s="5">
         <f>SUM(L3,L9)</f>
-        <v>28639.98</v>
+        <v>27728.309999999998</v>
       </c>
       <c r="S4" s="49">
         <v>42783</v>
@@ -1780,7 +1824,7 @@
       </c>
       <c r="AZ4" s="64">
         <f>(SUM((AO3:AO520)))-(SUM((AS3:AS520)))</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="BA4" s="64"/>
     </row>
@@ -1910,7 +1954,7 @@
       </c>
       <c r="L6" s="54">
         <f>(SUM((Q11:Q500),(V3:V520)))-(SUM(E11:E500))</f>
-        <v>985</v>
+        <v>977</v>
       </c>
       <c r="M6" s="32"/>
       <c r="N6" s="32"/>
@@ -2471,6 +2515,7 @@
       <c r="B11" t="s">
         <v>53</v>
       </c>
+      <c r="C11" s="40"/>
       <c r="D11" s="12">
         <v>4390</v>
       </c>
@@ -4311,7 +4356,7 @@
       </c>
       <c r="V25" s="43">
         <f t="shared" si="3"/>
-        <v>54.5</v>
+        <v>-245.5</v>
       </c>
       <c r="W25" s="52">
         <v>75</v>
@@ -4319,7 +4364,13 @@
       <c r="X25" s="52"/>
       <c r="Z25" s="53">
         <f t="shared" si="0"/>
-        <v>20.5</v>
+        <v>320.5</v>
+      </c>
+      <c r="AA25">
+        <v>250</v>
+      </c>
+      <c r="AB25" t="s">
+        <v>190</v>
       </c>
       <c r="AC25" t="s">
         <v>192</v>
@@ -4356,19 +4407,25 @@
       </c>
       <c r="AN25">
         <f t="shared" si="6"/>
-        <v>10.5</v>
+        <v>60.5</v>
       </c>
       <c r="AO25">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="AP25" s="40">
         <v>0</v>
       </c>
       <c r="AQ25">
         <v>0</v>
+      </c>
+      <c r="AR25">
+        <v>2</v>
       </c>
       <c r="AS25">
         <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="AT25">
         <v>0</v>
       </c>
       <c r="AU25">
@@ -4376,7 +4433,7 @@
         <v>0</v>
       </c>
       <c r="AV25">
-        <v>10.5</v>
+        <v>20.5</v>
       </c>
     </row>
     <row r="26" spans="1:57" x14ac:dyDescent="0.25">
@@ -4417,32 +4474,52 @@
       <c r="S26" s="49">
         <v>42805</v>
       </c>
-      <c r="T26" s="50"/>
-      <c r="U26" s="51"/>
+      <c r="T26" s="50" t="s">
+        <v>100</v>
+      </c>
+      <c r="U26" s="51" t="s">
+        <v>193</v>
+      </c>
       <c r="V26" s="43">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="W26" s="52"/>
-      <c r="X26" s="52"/>
+        <v>-190</v>
+      </c>
+      <c r="W26" s="52">
+        <v>300</v>
+      </c>
+      <c r="X26" s="52">
+        <v>500</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>194</v>
+      </c>
       <c r="Z26" s="53">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>990</v>
+      </c>
+      <c r="AA26">
+        <v>200</v>
+      </c>
+      <c r="AB26" t="s">
+        <v>195</v>
+      </c>
+      <c r="AC26" t="s">
+        <v>196</v>
       </c>
       <c r="AD26">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="AE26">
-        <v>0</v>
+        <v>290</v>
       </c>
       <c r="AF26">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AG26">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AH26">
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="AI26">
         <v>0</v>
@@ -4463,12 +4540,30 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="AO26">
+        <v>0</v>
+      </c>
+      <c r="AP26">
+        <v>0</v>
+      </c>
+      <c r="AQ26">
+        <v>0</v>
+      </c>
+      <c r="AR26">
+        <v>4</v>
+      </c>
       <c r="AS26">
         <f t="shared" si="7"/>
+        <v>20</v>
+      </c>
+      <c r="AT26">
         <v>0</v>
       </c>
       <c r="AU26">
         <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AV26">
         <v>0</v>
       </c>
     </row>
@@ -4509,18 +4604,33 @@
       <c r="S27" s="49">
         <v>42806</v>
       </c>
-      <c r="T27" s="50"/>
-      <c r="U27" s="51"/>
+      <c r="T27" s="50" t="s">
+        <v>108</v>
+      </c>
+      <c r="U27" s="51" t="s">
+        <v>200</v>
+      </c>
       <c r="V27" s="43">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="W27" s="52"/>
+        <v>50</v>
+      </c>
+      <c r="W27" s="52">
+        <v>50</v>
+      </c>
       <c r="X27" s="52"/>
+      <c r="Y27" t="s">
+        <v>201</v>
+      </c>
       <c r="Z27" s="53">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AA27">
+        <v>0</v>
+      </c>
+      <c r="AB27" t="s">
+        <v>145</v>
+      </c>
       <c r="AD27">
         <v>0</v>
       </c>
@@ -4555,18 +4665,41 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="AO27">
+        <v>0</v>
+      </c>
+      <c r="AP27">
+        <v>0</v>
+      </c>
+      <c r="AQ27">
+        <v>0</v>
+      </c>
+      <c r="AR27">
+        <v>0</v>
+      </c>
       <c r="AS27">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
+      <c r="AT27">
+        <v>0</v>
+      </c>
       <c r="AU27">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
+      <c r="AV27">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A28" s="34">
+        <v>42804</v>
+      </c>
       <c r="C28" s="13"/>
-      <c r="D28" s="12"/>
+      <c r="D28" s="12">
+        <v>161.15</v>
+      </c>
       <c r="E28" s="14"/>
       <c r="G28" s="60">
         <v>42789</v>
@@ -4587,28 +4720,47 @@
       </c>
       <c r="N28" s="59"/>
       <c r="O28" s="59"/>
-      <c r="P28" s="59"/>
+      <c r="P28" s="59" t="s">
+        <v>208</v>
+      </c>
       <c r="Q28" s="39"/>
       <c r="S28" s="49">
         <v>42807</v>
       </c>
-      <c r="T28" s="50"/>
-      <c r="U28" s="51"/>
+      <c r="T28" s="50" t="s">
+        <v>109</v>
+      </c>
+      <c r="U28" s="51" t="s">
+        <v>202</v>
+      </c>
       <c r="V28" s="43">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="W28" s="52"/>
-      <c r="X28" s="52"/>
+        <v>347.5</v>
+      </c>
+      <c r="W28" s="52">
+        <v>175</v>
+      </c>
+      <c r="X28" s="52">
+        <v>220</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>205</v>
+      </c>
       <c r="Z28" s="53">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>47.5</v>
+      </c>
+      <c r="AA28" s="40">
+        <v>0</v>
+      </c>
+      <c r="AC28" t="s">
+        <v>207</v>
       </c>
       <c r="AD28">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AE28">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AF28">
         <v>0</v>
@@ -4636,20 +4788,46 @@
       </c>
       <c r="AN28">
         <f t="shared" si="6"/>
+        <v>35.5</v>
+      </c>
+      <c r="AO28">
+        <v>0</v>
+      </c>
+      <c r="AP28">
+        <v>2</v>
+      </c>
+      <c r="AQ28">
+        <v>0</v>
+      </c>
+      <c r="AR28">
         <v>0</v>
       </c>
       <c r="AS28">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="AT28">
+        <v>4</v>
       </c>
       <c r="AU28">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="AV28">
+        <v>15.5</v>
       </c>
     </row>
     <row r="29" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A29" s="34">
+        <v>42804</v>
+      </c>
+      <c r="B29" t="s">
+        <v>197</v>
+      </c>
       <c r="C29" s="13"/>
-      <c r="D29" s="12"/>
+      <c r="D29" s="12">
+        <v>142.72999999999999</v>
+      </c>
       <c r="E29" s="14"/>
       <c r="G29" s="60">
         <v>42794</v>
@@ -4675,17 +4853,28 @@
       <c r="S29" s="49">
         <v>42808</v>
       </c>
-      <c r="T29" s="50"/>
-      <c r="U29" s="51"/>
+      <c r="T29" s="50" t="s">
+        <v>115</v>
+      </c>
+      <c r="U29" s="51" t="s">
+        <v>206</v>
+      </c>
       <c r="V29" s="43">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="W29" s="52"/>
-      <c r="X29" s="52"/>
+        <v>84.5</v>
+      </c>
+      <c r="W29" s="52">
+        <v>75</v>
+      </c>
+      <c r="X29" s="52">
+        <v>20</v>
+      </c>
+      <c r="Y29" t="s">
+        <v>204</v>
+      </c>
       <c r="Z29" s="53">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10.5</v>
       </c>
       <c r="AD29">
         <v>0</v>
@@ -4719,7 +4908,7 @@
       </c>
       <c r="AN29">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>10.5</v>
       </c>
       <c r="AS29">
         <f t="shared" si="7"/>
@@ -4729,10 +4918,21 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
+      <c r="AV29">
+        <v>10.5</v>
+      </c>
     </row>
     <row r="30" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A30" s="34">
+        <v>42805</v>
+      </c>
+      <c r="B30" t="s">
+        <v>198</v>
+      </c>
       <c r="C30" s="13"/>
-      <c r="D30" s="12"/>
+      <c r="D30" s="12">
+        <v>201</v>
+      </c>
       <c r="E30" s="14"/>
       <c r="G30" s="60">
         <v>42795</v>
@@ -4761,7 +4961,7 @@
       </c>
       <c r="T30" s="50"/>
       <c r="U30" s="51"/>
-      <c r="V30" s="43">
+      <c r="V30" s="85">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4816,8 +5016,16 @@
       </c>
     </row>
     <row r="31" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A31" s="34">
+        <v>42805</v>
+      </c>
+      <c r="B31" t="s">
+        <v>199</v>
+      </c>
       <c r="C31" s="13"/>
-      <c r="D31" s="12"/>
+      <c r="D31" s="12">
+        <v>52.79</v>
+      </c>
       <c r="E31" s="14"/>
       <c r="G31" s="59"/>
       <c r="H31" s="59"/>
@@ -4891,8 +5099,16 @@
       </c>
     </row>
     <row r="32" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A32" s="34">
+        <v>42807</v>
+      </c>
+      <c r="B32" t="s">
+        <v>203</v>
+      </c>
       <c r="C32" s="13"/>
-      <c r="D32" s="12"/>
+      <c r="D32" s="12">
+        <v>354</v>
+      </c>
       <c r="E32" s="14"/>
       <c r="G32" s="59"/>
       <c r="H32" s="59"/>

</xml_diff>

<commit_message>
Finanzas del fin de semana
</commit_message>
<xml_diff>
--- a/Finanzas/Febrero_2017.xlsx
+++ b/Finanzas/Febrero_2017.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="227">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -614,9 +614,6 @@
     <t>Marco café</t>
   </si>
   <si>
-    <t>Maíz</t>
-  </si>
-  <si>
     <t>ADRI FEST</t>
   </si>
   <si>
@@ -624,9 +621,6 @@
   </si>
   <si>
     <t>Perro negro</t>
-  </si>
-  <si>
-    <t>Enigma Enana; Karaoke x2 +30 enana; Alambre noche; Coca enana; Karaoke Brandon</t>
   </si>
   <si>
     <t>??????</t>
@@ -682,12 +676,54 @@
   <si>
     <t>Edgar Zapata</t>
   </si>
+  <si>
+    <t>Jaime pago China</t>
+  </si>
+  <si>
+    <t>Fiesta Manu</t>
+  </si>
+  <si>
+    <t>Puente</t>
+  </si>
+  <si>
+    <t>Mariscos</t>
+  </si>
+  <si>
+    <t>CARNES :$</t>
+  </si>
+  <si>
+    <t>Martes</t>
+  </si>
+  <si>
+    <t>Hooters Juancho</t>
+  </si>
+  <si>
+    <t>Arizona</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yogurth </t>
+  </si>
+  <si>
+    <t>Coca</t>
+  </si>
+  <si>
+    <t>Mariscos (62)</t>
+  </si>
+  <si>
+    <t>Taxi; Starbucks (128)</t>
+  </si>
+  <si>
+    <t>Enigma Enana; Karaoke x2 +30 enana; Alambre noche; Coca enana (25); Karaoke Brandon</t>
+  </si>
+  <si>
+    <t>Maíz; Coca (No registrada)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -824,6 +860,14 @@
       <u/>
       <sz val="11"/>
       <color theme="8" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -993,7 +1037,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1135,6 +1179,8 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1432,7 +1478,7 @@
   <dimension ref="A1:BE964"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1848,7 +1894,7 @@
       </c>
       <c r="AZ4" s="64">
         <f>(SUM((AO3:AO520)))-(SUM((AS3:AS520)))</f>
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="BA4" s="64"/>
     </row>
@@ -1978,7 +2024,7 @@
       </c>
       <c r="L6" s="54">
         <f>(SUM((Q11:Q500),(V3:V520)))-(SUM(E11:E500))</f>
-        <v>838</v>
+        <v>319.5</v>
       </c>
       <c r="M6" s="32"/>
       <c r="N6" s="32"/>
@@ -4380,7 +4426,7 @@
       </c>
       <c r="V25" s="43">
         <f t="shared" si="3"/>
-        <v>-245.5</v>
+        <v>-257.5</v>
       </c>
       <c r="W25" s="52">
         <v>75</v>
@@ -4388,7 +4434,7 @@
       <c r="X25" s="52"/>
       <c r="Z25" s="53">
         <f t="shared" si="0"/>
-        <v>320.5</v>
+        <v>332.5</v>
       </c>
       <c r="AA25">
         <v>250</v>
@@ -4397,13 +4443,13 @@
         <v>190</v>
       </c>
       <c r="AC25" t="s">
-        <v>192</v>
+        <v>226</v>
       </c>
       <c r="AD25">
         <v>10</v>
       </c>
-      <c r="AE25">
-        <v>0</v>
+      <c r="AE25" s="91">
+        <v>12</v>
       </c>
       <c r="AF25">
         <v>0</v>
@@ -4502,11 +4548,11 @@
         <v>100</v>
       </c>
       <c r="U26" s="51" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="V26" s="43">
         <f t="shared" si="3"/>
-        <v>-190</v>
+        <v>-200</v>
       </c>
       <c r="W26" s="52">
         <v>300</v>
@@ -4515,20 +4561,20 @@
         <v>500</v>
       </c>
       <c r="Y26" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="Z26" s="53">
         <f t="shared" si="0"/>
-        <v>990</v>
+        <v>1000</v>
       </c>
       <c r="AA26">
         <v>200</v>
       </c>
       <c r="AB26" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="AC26" t="s">
-        <v>196</v>
+        <v>225</v>
       </c>
       <c r="AD26">
         <v>250</v>
@@ -4539,8 +4585,8 @@
       <c r="AF26">
         <v>100</v>
       </c>
-      <c r="AG26">
-        <v>20</v>
+      <c r="AG26" s="12">
+        <v>30</v>
       </c>
       <c r="AH26">
         <v>130</v>
@@ -4632,7 +4678,7 @@
         <v>108</v>
       </c>
       <c r="U27" s="51" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="V27" s="43">
         <f t="shared" si="3"/>
@@ -4643,7 +4689,7 @@
       </c>
       <c r="X27" s="52"/>
       <c r="Y27" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="Z27" s="53">
         <f t="shared" si="0"/>
@@ -4745,7 +4791,7 @@
       <c r="N28" s="59"/>
       <c r="O28" s="59"/>
       <c r="P28" s="59" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="Q28" s="39"/>
       <c r="S28" s="49">
@@ -4755,7 +4801,7 @@
         <v>109</v>
       </c>
       <c r="U28" s="51" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="V28" s="43">
         <f t="shared" si="3"/>
@@ -4768,7 +4814,7 @@
         <v>220</v>
       </c>
       <c r="Y28" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="Z28" s="53">
         <f t="shared" si="0"/>
@@ -4778,7 +4824,7 @@
         <v>0</v>
       </c>
       <c r="AC28" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="AD28">
         <v>6</v>
@@ -4846,7 +4892,7 @@
         <v>42804</v>
       </c>
       <c r="B29" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C29" s="13"/>
       <c r="D29" s="12">
@@ -4881,7 +4927,7 @@
         <v>115</v>
       </c>
       <c r="U29" s="51" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="V29" s="43">
         <f t="shared" si="3"/>
@@ -4894,7 +4940,7 @@
         <v>20</v>
       </c>
       <c r="Y29" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="Z29" s="53">
         <f t="shared" si="0"/>
@@ -4904,10 +4950,10 @@
         <v>50</v>
       </c>
       <c r="AB29" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="AC29" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="AD29">
         <v>43</v>
@@ -4975,7 +5021,7 @@
         <v>42805</v>
       </c>
       <c r="B30" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C30" s="13"/>
       <c r="D30" s="12">
@@ -5011,7 +5057,7 @@
         <v>122</v>
       </c>
       <c r="U30" s="51" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="V30" s="85">
         <f t="shared" si="3"/>
@@ -5032,7 +5078,7 @@
         <v>120</v>
       </c>
       <c r="AC30" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="AD30">
         <v>10</v>
@@ -5100,7 +5146,7 @@
         <v>42805</v>
       </c>
       <c r="B31" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C31" s="13"/>
       <c r="D31" s="12">
@@ -5124,14 +5170,14 @@
         <v>42810</v>
       </c>
       <c r="T31" s="50" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="U31" s="51" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="V31" s="43">
         <f t="shared" si="3"/>
-        <v>64.5</v>
+        <v>-149.5</v>
       </c>
       <c r="W31" s="52">
         <v>75</v>
@@ -5139,13 +5185,22 @@
       <c r="X31" s="52"/>
       <c r="Z31" s="53">
         <f t="shared" si="0"/>
-        <v>10.5</v>
+        <v>224.5</v>
+      </c>
+      <c r="AA31">
+        <v>0</v>
+      </c>
+      <c r="AB31" t="s">
+        <v>213</v>
+      </c>
+      <c r="AC31" t="s">
+        <v>224</v>
       </c>
       <c r="AD31">
-        <v>0</v>
-      </c>
-      <c r="AE31">
-        <v>0</v>
+        <v>60</v>
+      </c>
+      <c r="AE31" s="12">
+        <v>130</v>
       </c>
       <c r="AF31">
         <v>0</v>
@@ -5173,10 +5228,25 @@
       </c>
       <c r="AN31">
         <f t="shared" si="6"/>
-        <v>10.5</v>
+        <v>34.5</v>
+      </c>
+      <c r="AO31" s="92">
+        <v>20</v>
+      </c>
+      <c r="AP31">
+        <v>0</v>
+      </c>
+      <c r="AQ31">
+        <v>0</v>
+      </c>
+      <c r="AR31">
+        <v>1</v>
       </c>
       <c r="AS31">
         <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="AT31">
         <v>0</v>
       </c>
       <c r="AU31">
@@ -5184,7 +5254,7 @@
         <v>0</v>
       </c>
       <c r="AV31">
-        <v>10.5</v>
+        <v>14.5</v>
       </c>
     </row>
     <row r="32" spans="1:57" x14ac:dyDescent="0.25">
@@ -5192,7 +5262,7 @@
         <v>42807</v>
       </c>
       <c r="B32" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C32" s="13"/>
       <c r="D32" s="12">
@@ -5215,17 +5285,29 @@
       <c r="S32" s="49">
         <v>42811</v>
       </c>
-      <c r="T32" s="50"/>
-      <c r="U32" s="51"/>
+      <c r="T32" s="50" t="s">
+        <v>83</v>
+      </c>
+      <c r="U32" s="51" t="s">
+        <v>214</v>
+      </c>
       <c r="V32" s="43">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="W32" s="52"/>
+        <v>-410.5</v>
+      </c>
+      <c r="W32" s="52">
+        <v>75</v>
+      </c>
       <c r="X32" s="52"/>
       <c r="Z32" s="53">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>485.5</v>
+      </c>
+      <c r="AA32">
+        <v>450</v>
+      </c>
+      <c r="AB32" s="40" t="s">
+        <v>217</v>
       </c>
       <c r="AD32">
         <v>0</v>
@@ -5259,18 +5341,36 @@
       </c>
       <c r="AN32">
         <f t="shared" si="6"/>
+        <v>35.5</v>
+      </c>
+      <c r="AO32">
+        <v>0</v>
+      </c>
+      <c r="AP32">
+        <v>2</v>
+      </c>
+      <c r="AQ32">
+        <v>0</v>
+      </c>
+      <c r="AR32">
         <v>0</v>
       </c>
       <c r="AS32">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="AT32" s="12">
+        <v>1</v>
       </c>
       <c r="AU32">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="3:47" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="AV32">
+        <v>30.5</v>
+      </c>
+    </row>
+    <row r="33" spans="3:48" x14ac:dyDescent="0.25">
       <c r="C33" s="13"/>
       <c r="D33" s="12"/>
       <c r="E33" s="14"/>
@@ -5287,20 +5387,35 @@
       <c r="S33" s="49">
         <v>42812</v>
       </c>
-      <c r="T33" s="50"/>
-      <c r="U33" s="51"/>
+      <c r="T33" s="50" t="s">
+        <v>100</v>
+      </c>
+      <c r="U33" s="51" t="s">
+        <v>216</v>
+      </c>
       <c r="V33" s="43">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="W33" s="52"/>
+        <v>6</v>
+      </c>
+      <c r="W33" s="52">
+        <v>120</v>
+      </c>
       <c r="X33" s="52"/>
       <c r="Z33" s="53">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>114</v>
+      </c>
+      <c r="AA33" s="91">
+        <v>82</v>
+      </c>
+      <c r="AB33" t="s">
+        <v>223</v>
+      </c>
+      <c r="AC33" t="s">
+        <v>222</v>
       </c>
       <c r="AD33">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AE33">
         <v>0</v>
@@ -5331,18 +5446,36 @@
       </c>
       <c r="AN33">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="AO33">
+        <v>20</v>
+      </c>
+      <c r="AP33">
+        <v>0</v>
+      </c>
+      <c r="AQ33">
+        <v>0</v>
+      </c>
+      <c r="AR33">
+        <v>3</v>
       </c>
       <c r="AS33">
         <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="AT33">
         <v>0</v>
       </c>
       <c r="AU33">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="3:47" x14ac:dyDescent="0.25">
+      <c r="AV33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="3:48" x14ac:dyDescent="0.25">
       <c r="C34" s="13"/>
       <c r="D34" s="12"/>
       <c r="E34" s="14"/>
@@ -5359,18 +5492,30 @@
       <c r="S34" s="49">
         <v>42813</v>
       </c>
-      <c r="T34" s="50"/>
-      <c r="U34" s="51"/>
+      <c r="T34" s="50" t="s">
+        <v>108</v>
+      </c>
+      <c r="U34" s="51" t="s">
+        <v>198</v>
+      </c>
       <c r="V34" s="43">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="W34" s="52"/>
+      <c r="W34" s="52">
+        <v>0</v>
+      </c>
       <c r="X34" s="52"/>
       <c r="Z34" s="53">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AA34">
+        <v>0</v>
+      </c>
+      <c r="AB34" t="s">
+        <v>145</v>
+      </c>
       <c r="AD34">
         <v>0</v>
       </c>
@@ -5405,16 +5550,34 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="AO34">
+        <v>0</v>
+      </c>
+      <c r="AP34">
+        <v>0</v>
+      </c>
+      <c r="AQ34">
+        <v>0</v>
+      </c>
+      <c r="AR34">
+        <v>0</v>
+      </c>
       <c r="AS34">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
+      <c r="AT34">
+        <v>0</v>
+      </c>
       <c r="AU34">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="3:47" x14ac:dyDescent="0.25">
+      <c r="AV34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="3:48" x14ac:dyDescent="0.25">
       <c r="C35" s="13"/>
       <c r="D35" s="12"/>
       <c r="E35" s="14"/>
@@ -5431,20 +5594,35 @@
       <c r="S35" s="49">
         <v>42814</v>
       </c>
-      <c r="T35" s="50"/>
-      <c r="U35" s="51"/>
+      <c r="T35" s="50" t="s">
+        <v>109</v>
+      </c>
+      <c r="U35" s="51" t="s">
+        <v>215</v>
+      </c>
       <c r="V35" s="43">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="W35" s="52"/>
+        <v>39</v>
+      </c>
+      <c r="W35" s="52">
+        <v>100</v>
+      </c>
       <c r="X35" s="52"/>
       <c r="Z35" s="53">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>61</v>
+      </c>
+      <c r="AA35">
+        <v>0</v>
+      </c>
+      <c r="AB35" t="s">
+        <v>145</v>
+      </c>
+      <c r="AC35" t="s">
+        <v>220</v>
       </c>
       <c r="AD35">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="AE35">
         <v>0</v>
@@ -5475,18 +5653,36 @@
       </c>
       <c r="AN35">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>50</v>
+      </c>
+      <c r="AO35">
+        <v>40</v>
+      </c>
+      <c r="AP35">
+        <v>2</v>
+      </c>
+      <c r="AQ35">
+        <v>0</v>
+      </c>
+      <c r="AR35">
+        <v>2</v>
       </c>
       <c r="AS35">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>22</v>
+      </c>
+      <c r="AT35">
+        <v>2</v>
       </c>
       <c r="AU35">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="3:47" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="AV35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="3:48" x14ac:dyDescent="0.25">
       <c r="C36" s="13"/>
       <c r="D36" s="12"/>
       <c r="E36" s="14"/>
@@ -5503,20 +5699,37 @@
       <c r="S36" s="49">
         <v>42815</v>
       </c>
-      <c r="T36" s="50"/>
-      <c r="U36" s="51"/>
+      <c r="T36" s="50" t="s">
+        <v>218</v>
+      </c>
+      <c r="U36" s="51" t="s">
+        <v>219</v>
+      </c>
       <c r="V36" s="43">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="W36" s="52"/>
-      <c r="X36" s="52"/>
+        <v>83</v>
+      </c>
+      <c r="W36" s="52">
+        <v>75</v>
+      </c>
+      <c r="X36" s="52">
+        <v>80</v>
+      </c>
       <c r="Z36" s="53">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>72</v>
+      </c>
+      <c r="AA36">
+        <v>60</v>
+      </c>
+      <c r="AB36" t="s">
+        <v>207</v>
+      </c>
+      <c r="AC36" t="s">
+        <v>221</v>
       </c>
       <c r="AD36">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AE36">
         <v>0</v>
@@ -5558,7 +5771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="3:47" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:48" x14ac:dyDescent="0.25">
       <c r="C37" s="13"/>
       <c r="D37" s="12"/>
       <c r="E37" s="14"/>
@@ -5630,7 +5843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="3:47" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:48" x14ac:dyDescent="0.25">
       <c r="C38" s="13"/>
       <c r="D38" s="12"/>
       <c r="E38" s="14"/>
@@ -5702,7 +5915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="3:47" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:48" x14ac:dyDescent="0.25">
       <c r="C39" s="13"/>
       <c r="D39" s="12"/>
       <c r="E39" s="14"/>
@@ -5774,7 +5987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="3:47" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:48" x14ac:dyDescent="0.25">
       <c r="C40" s="13"/>
       <c r="D40" s="12"/>
       <c r="E40" s="14"/>
@@ -5846,7 +6059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="3:47" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:48" x14ac:dyDescent="0.25">
       <c r="C41" s="13"/>
       <c r="D41" s="12"/>
       <c r="E41" s="14"/>
@@ -5918,7 +6131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="3:47" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:48" x14ac:dyDescent="0.25">
       <c r="C42" s="13"/>
       <c r="D42" s="12"/>
       <c r="E42" s="14"/>
@@ -5990,7 +6203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="3:47" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:48" x14ac:dyDescent="0.25">
       <c r="C43" s="13"/>
       <c r="D43" s="12"/>
       <c r="E43" s="14"/>
@@ -6062,7 +6275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="3:47" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:48" x14ac:dyDescent="0.25">
       <c r="C44" s="13"/>
       <c r="D44" s="12"/>
       <c r="E44" s="14"/>
@@ -6134,7 +6347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="3:47" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:48" x14ac:dyDescent="0.25">
       <c r="C45" s="13"/>
       <c r="D45" s="12"/>
       <c r="E45" s="14"/>
@@ -6206,7 +6419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="3:47" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:48" x14ac:dyDescent="0.25">
       <c r="C46" s="13"/>
       <c r="D46" s="12"/>
       <c r="E46" s="14"/>
@@ -6278,7 +6491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="3:47" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:48" x14ac:dyDescent="0.25">
       <c r="C47" s="13"/>
       <c r="D47" s="12"/>
       <c r="E47" s="14"/>
@@ -6348,7 +6561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="3:47" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:48" x14ac:dyDescent="0.25">
       <c r="C48" s="13"/>
       <c r="D48" s="12"/>
       <c r="E48" s="14"/>

</xml_diff>

<commit_message>
Dia del reporte PAPIIT
</commit_message>
<xml_diff>
--- a/Finanzas/Febrero_2017.xlsx
+++ b/Finanzas/Febrero_2017.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="230">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -339,9 +339,6 @@
   </si>
   <si>
     <t>Efectivo 50</t>
-  </si>
-  <si>
-    <t>Ajuste de dinero no contado para que coincida con el efectivo en mi cartera</t>
   </si>
   <si>
     <t>Fui con Jaime a comer bistecates y a jugar videojuegos</t>
@@ -689,9 +686,6 @@
     <t>Mariscos</t>
   </si>
   <si>
-    <t>CARNES :$</t>
-  </si>
-  <si>
     <t>Martes</t>
   </si>
   <si>
@@ -701,29 +695,44 @@
     <t>Arizona</t>
   </si>
   <si>
-    <t xml:space="preserve">Yogurth </t>
-  </si>
-  <si>
     <t>Coca</t>
   </si>
   <si>
-    <t>Mariscos (62)</t>
+    <t>Maíz; Coca (No registrada)</t>
   </si>
   <si>
-    <t>Taxi; Starbucks (128)</t>
+    <t>Yogurth ; Prestamo Enana</t>
   </si>
   <si>
-    <t>Enigma Enana; Karaoke x2 +30 enana; Alambre noche; Coca enana (25); Karaoke Brandon</t>
+    <t>PAPIIT termino</t>
   </si>
   <si>
-    <t>Maíz; Coca (No registrada)</t>
+    <t xml:space="preserve">Mariscos </t>
+  </si>
+  <si>
+    <t>Enigma Enana; Karaoke x2 +30 enana; Alambre noche; Coca enana; Karaoke Brandon</t>
+  </si>
+  <si>
+    <t>Taxi; Starbucks</t>
+  </si>
+  <si>
+    <t>CARNES :3</t>
+  </si>
+  <si>
+    <t>Cooperacha café</t>
+  </si>
+  <si>
+    <t>Mamá para cortar cabello</t>
+  </si>
+  <si>
+    <t>Javs Invita Cumple</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -860,14 +869,6 @@
       <u/>
       <sz val="11"/>
       <color theme="8" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1037,7 +1038,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1179,7 +1180,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1506,7 +1506,7 @@
         <v>42782</v>
       </c>
       <c r="D1" s="82" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="P1" s="78"/>
       <c r="S1" s="46"/>
@@ -1641,10 +1641,10 @@
         <v>84</v>
       </c>
       <c r="AP2" s="62" t="s">
+        <v>180</v>
+      </c>
+      <c r="AQ2" s="62" t="s">
         <v>181</v>
-      </c>
-      <c r="AQ2" s="62" t="s">
-        <v>182</v>
       </c>
       <c r="AR2" s="62" t="s">
         <v>92</v>
@@ -1656,7 +1656,7 @@
         <v>86</v>
       </c>
       <c r="AU2" s="77" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AV2" s="62" t="s">
         <v>87</v>
@@ -1796,7 +1796,7 @@
       </c>
       <c r="N4" s="5">
         <f>SUM(L3,L9)</f>
-        <v>27728.309999999998</v>
+        <v>27878.309999999998</v>
       </c>
       <c r="S4" s="49">
         <v>42783</v>
@@ -1805,7 +1805,7 @@
         <v>83</v>
       </c>
       <c r="U4" s="51" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="V4" s="43">
         <f t="shared" ref="V4:V67" si="3">(SUM(W4,X4))-Z4</f>
@@ -1894,7 +1894,7 @@
       </c>
       <c r="AZ4" s="64">
         <f>(SUM((AO3:AO520)))-(SUM((AS3:AS520)))</f>
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="BA4" s="64"/>
     </row>
@@ -1922,11 +1922,11 @@
         <v>100</v>
       </c>
       <c r="U5" s="51" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="V5" s="43">
         <f t="shared" si="3"/>
-        <v>332.5</v>
+        <v>300</v>
       </c>
       <c r="W5" s="52">
         <v>120</v>
@@ -1939,7 +1939,7 @@
       </c>
       <c r="Z5" s="53">
         <f t="shared" si="0"/>
-        <v>-12.5</v>
+        <v>20</v>
       </c>
       <c r="AA5">
         <v>0</v>
@@ -1947,12 +1947,8 @@
       <c r="AB5" t="s">
         <v>101</v>
       </c>
-      <c r="AC5" s="69" t="s">
-        <v>105</v>
-      </c>
-      <c r="AD5" s="69">
-        <v>-32.5</v>
-      </c>
+      <c r="AC5" s="59"/>
+      <c r="AD5" s="59"/>
       <c r="AE5">
         <v>0</v>
       </c>
@@ -2024,7 +2020,7 @@
       </c>
       <c r="L6" s="54">
         <f>(SUM((Q11:Q500),(V3:V520)))-(SUM(E11:E500))</f>
-        <v>319.5</v>
+        <v>234</v>
       </c>
       <c r="M6" s="32"/>
       <c r="N6" s="32"/>
@@ -2032,10 +2028,10 @@
         <v>42785</v>
       </c>
       <c r="T6" s="50" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="U6" s="74" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="V6" s="43">
         <f t="shared" si="3"/>
@@ -2046,7 +2042,7 @@
       </c>
       <c r="X6" s="52"/>
       <c r="Y6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Z6" s="53">
         <f t="shared" si="0"/>
@@ -2056,7 +2052,7 @@
         <v>0</v>
       </c>
       <c r="AB6" s="40" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AD6">
         <v>0</v>
@@ -2135,10 +2131,10 @@
         <v>42786</v>
       </c>
       <c r="T7" s="50" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="U7" s="51" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="V7" s="43">
         <f t="shared" si="3"/>
@@ -2159,7 +2155,7 @@
         <v>97</v>
       </c>
       <c r="AC7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AD7">
         <v>10</v>
@@ -2229,10 +2225,10 @@
         <v>42787</v>
       </c>
       <c r="T8" s="50" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="U8" s="51" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="V8" s="43">
         <f t="shared" si="3"/>
@@ -2245,7 +2241,7 @@
         <v>9</v>
       </c>
       <c r="Y8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="Z8" s="53">
         <f t="shared" si="0"/>
@@ -2255,10 +2251,10 @@
         <v>70</v>
       </c>
       <c r="AB8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AC8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AD8">
         <v>9</v>
@@ -2340,7 +2336,7 @@
       </c>
       <c r="L9" s="15">
         <f>SUM(L11:L500)</f>
-        <v>23829</v>
+        <v>23979</v>
       </c>
       <c r="N9" s="35" t="s">
         <v>56</v>
@@ -2352,10 +2348,10 @@
         <v>42788</v>
       </c>
       <c r="T9" s="50" t="s">
+        <v>121</v>
+      </c>
+      <c r="U9" s="51" t="s">
         <v>122</v>
-      </c>
-      <c r="U9" s="51" t="s">
-        <v>123</v>
       </c>
       <c r="V9" s="43">
         <f t="shared" si="3"/>
@@ -2366,7 +2362,7 @@
         <v>500</v>
       </c>
       <c r="Y9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="Z9" s="53">
         <f t="shared" si="0"/>
@@ -2376,10 +2372,10 @@
         <v>100</v>
       </c>
       <c r="AB9" t="s">
+        <v>124</v>
+      </c>
+      <c r="AC9" t="s">
         <v>125</v>
-      </c>
-      <c r="AC9" t="s">
-        <v>126</v>
       </c>
       <c r="AD9">
         <v>50</v>
@@ -2496,7 +2492,7 @@
         <v>63</v>
       </c>
       <c r="U10" s="51" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="V10" s="43">
         <f t="shared" si="3"/>
@@ -2512,10 +2508,10 @@
         <v>0</v>
       </c>
       <c r="AB10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AC10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AD10">
         <v>25</v>
@@ -2628,7 +2624,7 @@
         <v>83</v>
       </c>
       <c r="U11" s="51" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="V11" s="43">
         <f t="shared" si="3"/>
@@ -2644,10 +2640,10 @@
         <v>24</v>
       </c>
       <c r="AB11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AC11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="AD11">
         <v>10</v>
@@ -2746,7 +2742,7 @@
         <v>57</v>
       </c>
       <c r="P12" s="59" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="Q12" s="39">
         <v>465</v>
@@ -2758,7 +2754,7 @@
         <v>100</v>
       </c>
       <c r="U12" s="51" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V12" s="43">
         <f t="shared" si="3"/>
@@ -2776,7 +2772,7 @@
         <v>70</v>
       </c>
       <c r="AB12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AD12">
         <v>0</v>
@@ -2872,10 +2868,10 @@
         <v>42798</v>
       </c>
       <c r="O13" s="59" t="s">
+        <v>170</v>
+      </c>
+      <c r="P13" s="59" t="s">
         <v>171</v>
-      </c>
-      <c r="P13" s="59" t="s">
-        <v>172</v>
       </c>
       <c r="Q13" s="39">
         <v>600</v>
@@ -2884,10 +2880,10 @@
         <v>42792</v>
       </c>
       <c r="T13" s="50" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="U13" s="51" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="V13" s="43">
         <f t="shared" si="3"/>
@@ -2898,7 +2894,7 @@
         <v>350</v>
       </c>
       <c r="Y13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Z13" s="53">
         <f t="shared" si="0"/>
@@ -2908,10 +2904,10 @@
         <v>0</v>
       </c>
       <c r="AB13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AC13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AD13">
         <v>20</v>
@@ -3010,7 +3006,7 @@
         <v>29</v>
       </c>
       <c r="P14" s="59" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="Q14" s="39">
         <v>500</v>
@@ -3019,10 +3015,10 @@
         <v>42793</v>
       </c>
       <c r="T14" s="50" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="U14" s="51" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="V14" s="43">
         <f t="shared" si="3"/>
@@ -3040,10 +3036,10 @@
         <v>40</v>
       </c>
       <c r="AB14" t="s">
+        <v>147</v>
+      </c>
+      <c r="AC14" t="s">
         <v>148</v>
-      </c>
-      <c r="AC14" t="s">
-        <v>149</v>
       </c>
       <c r="AD14">
         <v>8</v>
@@ -3111,7 +3107,7 @@
         <v>42787</v>
       </c>
       <c r="B15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C15" s="13"/>
       <c r="D15" s="80">
@@ -3142,7 +3138,7 @@
         <v>57</v>
       </c>
       <c r="P15" s="59" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="Q15" s="39">
         <v>400</v>
@@ -3151,10 +3147,10 @@
         <v>42794</v>
       </c>
       <c r="T15" s="50" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="U15" s="74" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="V15" s="43">
         <f t="shared" si="3"/>
@@ -3167,7 +3163,7 @@
         <v>40</v>
       </c>
       <c r="Y15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="Z15" s="53">
         <f t="shared" si="0"/>
@@ -3180,7 +3176,7 @@
         <v>97</v>
       </c>
       <c r="AC15" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AD15">
         <v>10</v>
@@ -3248,7 +3244,7 @@
         <v>42790</v>
       </c>
       <c r="B16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C16" s="13"/>
       <c r="D16" s="80">
@@ -3280,10 +3276,10 @@
         <v>42795</v>
       </c>
       <c r="T16" s="50" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="U16" s="51" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="V16" s="43">
         <f t="shared" si="3"/>
@@ -3296,7 +3292,7 @@
         <v>50</v>
       </c>
       <c r="Y16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="Z16" s="84">
         <f t="shared" si="0"/>
@@ -3306,10 +3302,10 @@
         <v>70</v>
       </c>
       <c r="AB16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AC16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="AD16" s="19">
         <v>20</v>
@@ -3378,7 +3374,7 @@
         <v>42790</v>
       </c>
       <c r="B17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C17" s="13"/>
       <c r="D17" s="12">
@@ -3413,7 +3409,7 @@
         <v>63</v>
       </c>
       <c r="U17" s="51" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="V17" s="43">
         <f t="shared" si="3"/>
@@ -3431,10 +3427,10 @@
         <v>40</v>
       </c>
       <c r="AB17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AC17" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="AD17">
         <v>3</v>
@@ -3501,10 +3497,10 @@
     </row>
     <row r="18" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B18" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C18" s="13"/>
       <c r="D18" s="12">
@@ -3540,7 +3536,7 @@
         <v>83</v>
       </c>
       <c r="U18" s="51" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="V18" s="85">
         <f t="shared" si="3"/>
@@ -3558,10 +3554,10 @@
         <v>0</v>
       </c>
       <c r="AB18" t="s">
+        <v>165</v>
+      </c>
+      <c r="AC18" t="s">
         <v>166</v>
-      </c>
-      <c r="AC18" t="s">
-        <v>167</v>
       </c>
       <c r="AD18">
         <v>80</v>
@@ -3629,7 +3625,7 @@
         <v>42793</v>
       </c>
       <c r="B19" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C19" s="13"/>
       <c r="D19" s="12"/>
@@ -3664,7 +3660,7 @@
         <v>100</v>
       </c>
       <c r="U19" s="51" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="V19" s="43">
         <f t="shared" si="3"/>
@@ -3677,7 +3673,7 @@
         <v>40</v>
       </c>
       <c r="Y19" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="Z19" s="53">
         <f t="shared" si="0"/>
@@ -3687,10 +3683,10 @@
         <v>30</v>
       </c>
       <c r="AB19" t="s">
+        <v>168</v>
+      </c>
+      <c r="AC19" t="s">
         <v>169</v>
-      </c>
-      <c r="AC19" t="s">
-        <v>170</v>
       </c>
       <c r="AD19">
         <v>6</v>
@@ -3759,7 +3755,7 @@
         <v>42794</v>
       </c>
       <c r="B20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C20" s="13"/>
       <c r="D20" s="73">
@@ -3791,10 +3787,10 @@
         <v>42799</v>
       </c>
       <c r="T20" s="50" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="U20" s="51" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="V20" s="43">
         <f t="shared" si="3"/>
@@ -3807,7 +3803,7 @@
         <v>15</v>
       </c>
       <c r="Y20" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="Z20" s="53">
         <f t="shared" si="0"/>
@@ -3817,10 +3813,10 @@
         <v>100</v>
       </c>
       <c r="AB20" t="s">
+        <v>176</v>
+      </c>
+      <c r="AC20" t="s">
         <v>177</v>
-      </c>
-      <c r="AC20" t="s">
-        <v>178</v>
       </c>
       <c r="AD20">
         <v>150</v>
@@ -3887,7 +3883,7 @@
         <v>42794</v>
       </c>
       <c r="B21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C21" s="87"/>
       <c r="D21" s="12">
@@ -3919,10 +3915,10 @@
         <v>42800</v>
       </c>
       <c r="T21" s="50" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="U21" s="51" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="V21" s="43">
         <f t="shared" si="3"/>
@@ -4008,7 +4004,7 @@
         <v>42798</v>
       </c>
       <c r="B22" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C22" s="13"/>
       <c r="D22" s="12">
@@ -4042,10 +4038,10 @@
         <v>42801</v>
       </c>
       <c r="T22" s="50" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="U22" s="51" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="V22" s="43">
         <f t="shared" si="3"/>
@@ -4063,7 +4059,7 @@
         <v>0</v>
       </c>
       <c r="AC22" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AD22" s="40">
         <v>50</v>
@@ -4131,7 +4127,7 @@
         <v>42798</v>
       </c>
       <c r="B23" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C23" s="13"/>
       <c r="D23" s="73">
@@ -4165,10 +4161,10 @@
         <v>42802</v>
       </c>
       <c r="T23" s="50" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="U23" s="51" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="V23" s="43">
         <f t="shared" si="3"/>
@@ -4181,7 +4177,7 @@
         <v>50</v>
       </c>
       <c r="Y23" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="Z23" s="53">
         <f t="shared" si="0"/>
@@ -4191,10 +4187,10 @@
         <v>110</v>
       </c>
       <c r="AB23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AC23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AD23">
         <v>7.5</v>
@@ -4262,7 +4258,7 @@
         <v>42800</v>
       </c>
       <c r="B24" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C24" s="13"/>
       <c r="D24" s="12"/>
@@ -4298,7 +4294,7 @@
         <v>63</v>
       </c>
       <c r="U24" s="51" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="V24" s="43">
         <f t="shared" si="3"/>
@@ -4316,7 +4312,7 @@
         <v>70</v>
       </c>
       <c r="AB24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AD24">
         <v>0</v>
@@ -4384,7 +4380,7 @@
         <v>42802</v>
       </c>
       <c r="B25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C25" s="13"/>
       <c r="D25" s="12">
@@ -4422,7 +4418,7 @@
         <v>83</v>
       </c>
       <c r="U25" s="51" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="V25" s="43">
         <f t="shared" si="3"/>
@@ -4440,10 +4436,10 @@
         <v>250</v>
       </c>
       <c r="AB25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AC25" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="AD25">
         <v>10</v>
@@ -4511,7 +4507,7 @@
         <v>42802</v>
       </c>
       <c r="B26" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C26" s="13"/>
       <c r="D26" s="12">
@@ -4548,11 +4544,11 @@
         <v>100</v>
       </c>
       <c r="U26" s="51" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="V26" s="43">
         <f t="shared" si="3"/>
-        <v>-200</v>
+        <v>-190</v>
       </c>
       <c r="W26" s="52">
         <v>300</v>
@@ -4561,20 +4557,20 @@
         <v>500</v>
       </c>
       <c r="Y26" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="Z26" s="53">
         <f t="shared" si="0"/>
-        <v>1000</v>
+        <v>990</v>
       </c>
       <c r="AA26">
         <v>200</v>
       </c>
       <c r="AB26" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AC26" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="AD26">
         <v>250</v>
@@ -4585,8 +4581,8 @@
       <c r="AF26">
         <v>100</v>
       </c>
-      <c r="AG26" s="12">
-        <v>30</v>
+      <c r="AG26" s="91">
+        <v>20</v>
       </c>
       <c r="AH26">
         <v>130</v>
@@ -4642,7 +4638,7 @@
         <v>42802</v>
       </c>
       <c r="B27" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C27" s="13"/>
       <c r="D27" s="12">
@@ -4675,10 +4671,10 @@
         <v>42806</v>
       </c>
       <c r="T27" s="50" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="U27" s="51" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="V27" s="43">
         <f t="shared" si="3"/>
@@ -4689,7 +4685,7 @@
       </c>
       <c r="X27" s="52"/>
       <c r="Y27" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="Z27" s="53">
         <f t="shared" si="0"/>
@@ -4699,7 +4695,7 @@
         <v>0</v>
       </c>
       <c r="AB27" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AD27">
         <v>0</v>
@@ -4775,10 +4771,10 @@
         <v>42789</v>
       </c>
       <c r="H28" s="59" t="s">
+        <v>127</v>
+      </c>
+      <c r="I28" s="59" t="s">
         <v>128</v>
-      </c>
-      <c r="I28" s="59" t="s">
-        <v>129</v>
       </c>
       <c r="J28" s="24">
         <v>100</v>
@@ -4791,17 +4787,17 @@
       <c r="N28" s="59"/>
       <c r="O28" s="59"/>
       <c r="P28" s="59" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q28" s="39"/>
       <c r="S28" s="49">
         <v>42807</v>
       </c>
       <c r="T28" s="50" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="U28" s="51" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="V28" s="43">
         <f t="shared" si="3"/>
@@ -4814,7 +4810,7 @@
         <v>220</v>
       </c>
       <c r="Y28" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="Z28" s="53">
         <f t="shared" si="0"/>
@@ -4824,7 +4820,7 @@
         <v>0</v>
       </c>
       <c r="AC28" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="AD28">
         <v>6</v>
@@ -4892,7 +4888,7 @@
         <v>42804</v>
       </c>
       <c r="B29" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C29" s="13"/>
       <c r="D29" s="12">
@@ -4903,10 +4899,10 @@
         <v>42794</v>
       </c>
       <c r="H29" s="59" t="s">
+        <v>153</v>
+      </c>
+      <c r="I29" s="83" t="s">
         <v>154</v>
-      </c>
-      <c r="I29" s="83" t="s">
-        <v>155</v>
       </c>
       <c r="J29" s="24">
         <v>10</v>
@@ -4924,10 +4920,10 @@
         <v>42808</v>
       </c>
       <c r="T29" s="50" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="U29" s="51" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="V29" s="43">
         <f t="shared" si="3"/>
@@ -4940,7 +4936,7 @@
         <v>20</v>
       </c>
       <c r="Y29" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="Z29" s="53">
         <f t="shared" si="0"/>
@@ -4950,10 +4946,10 @@
         <v>50</v>
       </c>
       <c r="AB29" t="s">
+        <v>206</v>
+      </c>
+      <c r="AC29" t="s">
         <v>207</v>
-      </c>
-      <c r="AC29" t="s">
-        <v>208</v>
       </c>
       <c r="AD29">
         <v>43</v>
@@ -5021,7 +5017,7 @@
         <v>42805</v>
       </c>
       <c r="B30" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C30" s="13"/>
       <c r="D30" s="12">
@@ -5032,16 +5028,16 @@
         <v>42795</v>
       </c>
       <c r="H30" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I30" s="59" t="s">
         <v>159</v>
-      </c>
-      <c r="I30" s="59" t="s">
-        <v>160</v>
       </c>
       <c r="J30" s="24">
         <v>20</v>
       </c>
       <c r="K30" s="75" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L30" s="21">
         <v>0</v>
@@ -5054,10 +5050,10 @@
         <v>42809</v>
       </c>
       <c r="T30" s="50" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="U30" s="51" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="V30" s="85">
         <f t="shared" si="3"/>
@@ -5075,10 +5071,10 @@
         <v>70</v>
       </c>
       <c r="AB30" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AC30" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AD30">
         <v>10</v>
@@ -5146,21 +5142,29 @@
         <v>42805</v>
       </c>
       <c r="B31" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C31" s="13"/>
       <c r="D31" s="12">
         <v>52.79</v>
       </c>
       <c r="E31" s="14"/>
-      <c r="G31" s="59"/>
-      <c r="H31" s="59"/>
-      <c r="I31" s="59"/>
-      <c r="J31" s="24"/>
+      <c r="G31" s="60">
+        <v>42816</v>
+      </c>
+      <c r="H31" s="59" t="s">
+        <v>28</v>
+      </c>
+      <c r="I31" s="59" t="s">
+        <v>217</v>
+      </c>
+      <c r="J31" s="24">
+        <v>150</v>
+      </c>
       <c r="K31" s="23"/>
       <c r="L31" s="21">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="N31" s="59"/>
       <c r="O31" s="59"/>
@@ -5170,14 +5174,14 @@
         <v>42810</v>
       </c>
       <c r="T31" s="50" t="s">
+        <v>210</v>
+      </c>
+      <c r="U31" s="51" t="s">
         <v>211</v>
-      </c>
-      <c r="U31" s="51" t="s">
-        <v>212</v>
       </c>
       <c r="V31" s="43">
         <f t="shared" si="3"/>
-        <v>-149.5</v>
+        <v>-147.5</v>
       </c>
       <c r="W31" s="52">
         <v>75</v>
@@ -5185,22 +5189,22 @@
       <c r="X31" s="52"/>
       <c r="Z31" s="53">
         <f t="shared" si="0"/>
-        <v>224.5</v>
+        <v>222.5</v>
       </c>
       <c r="AA31">
         <v>0</v>
       </c>
       <c r="AB31" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="AC31" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="AD31">
         <v>60</v>
       </c>
-      <c r="AE31" s="12">
-        <v>130</v>
+      <c r="AE31" s="91">
+        <v>128</v>
       </c>
       <c r="AF31">
         <v>0</v>
@@ -5230,7 +5234,7 @@
         <f t="shared" si="6"/>
         <v>34.5</v>
       </c>
-      <c r="AO31" s="92">
+      <c r="AO31" s="91">
         <v>20</v>
       </c>
       <c r="AP31">
@@ -5262,7 +5266,7 @@
         <v>42807</v>
       </c>
       <c r="B32" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C32" s="13"/>
       <c r="D32" s="12">
@@ -5289,7 +5293,7 @@
         <v>83</v>
       </c>
       <c r="U32" s="51" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="V32" s="43">
         <f t="shared" si="3"/>
@@ -5307,7 +5311,7 @@
         <v>450</v>
       </c>
       <c r="AB32" s="40" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="AD32">
         <v>0</v>
@@ -5391,11 +5395,11 @@
         <v>100</v>
       </c>
       <c r="U33" s="51" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="V33" s="43">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="W33" s="52">
         <v>120</v>
@@ -5403,16 +5407,16 @@
       <c r="X33" s="52"/>
       <c r="Z33" s="53">
         <f t="shared" si="0"/>
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="AA33" s="91">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="AB33" t="s">
         <v>223</v>
       </c>
       <c r="AC33" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="AD33">
         <v>12</v>
@@ -5493,10 +5497,10 @@
         <v>42813</v>
       </c>
       <c r="T34" s="50" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="U34" s="51" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="V34" s="43">
         <f t="shared" si="3"/>
@@ -5514,7 +5518,7 @@
         <v>0</v>
       </c>
       <c r="AB34" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AD34">
         <v>0</v>
@@ -5595,14 +5599,14 @@
         <v>42814</v>
       </c>
       <c r="T35" s="50" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="U35" s="51" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="V35" s="43">
         <f t="shared" si="3"/>
-        <v>39</v>
+        <v>79</v>
       </c>
       <c r="W35" s="52">
         <v>100</v>
@@ -5610,16 +5614,16 @@
       <c r="X35" s="52"/>
       <c r="Z35" s="53">
         <f t="shared" si="0"/>
-        <v>61</v>
+        <v>21</v>
       </c>
       <c r="AA35">
         <v>0</v>
       </c>
       <c r="AB35" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AC35" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="AD35">
         <v>11</v>
@@ -5653,23 +5657,23 @@
       </c>
       <c r="AN35">
         <f t="shared" si="6"/>
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="AO35">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="AP35">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AQ35">
         <v>0</v>
       </c>
       <c r="AR35">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AS35">
         <f t="shared" si="7"/>
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="AT35">
         <v>2</v>
@@ -5700,14 +5704,14 @@
         <v>42815</v>
       </c>
       <c r="T36" s="50" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="U36" s="51" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="V36" s="43">
         <f t="shared" si="3"/>
-        <v>83</v>
+        <v>-122.5</v>
       </c>
       <c r="W36" s="52">
         <v>75</v>
@@ -5717,13 +5721,13 @@
       </c>
       <c r="Z36" s="53">
         <f t="shared" si="0"/>
-        <v>72</v>
+        <v>277.5</v>
       </c>
       <c r="AA36">
         <v>60</v>
       </c>
       <c r="AB36" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AC36" t="s">
         <v>221</v>
@@ -5731,8 +5735,8 @@
       <c r="AD36">
         <v>12</v>
       </c>
-      <c r="AE36">
-        <v>0</v>
+      <c r="AE36" s="19">
+        <v>150</v>
       </c>
       <c r="AF36">
         <v>0</v>
@@ -5760,15 +5764,33 @@
       </c>
       <c r="AN36">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>55.5</v>
+      </c>
+      <c r="AO36">
+        <v>40</v>
+      </c>
+      <c r="AP36">
+        <v>2</v>
+      </c>
+      <c r="AQ36">
+        <v>0</v>
+      </c>
+      <c r="AR36">
+        <v>2</v>
       </c>
       <c r="AS36">
         <f t="shared" si="7"/>
+        <v>22</v>
+      </c>
+      <c r="AT36">
         <v>0</v>
       </c>
       <c r="AU36">
         <f t="shared" si="4"/>
         <v>0</v>
+      </c>
+      <c r="AV36">
+        <v>15.5</v>
       </c>
     </row>
     <row r="37" spans="3:48" x14ac:dyDescent="0.25">
@@ -5788,20 +5810,40 @@
       <c r="S37" s="49">
         <v>42816</v>
       </c>
-      <c r="T37" s="50"/>
-      <c r="U37" s="51"/>
+      <c r="T37" s="50" t="s">
+        <v>121</v>
+      </c>
+      <c r="U37" s="51" t="s">
+        <v>222</v>
+      </c>
       <c r="V37" s="43">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="W37" s="52"/>
-      <c r="X37" s="52"/>
+        <v>80.5</v>
+      </c>
+      <c r="W37" s="52">
+        <v>105</v>
+      </c>
+      <c r="X37" s="52">
+        <v>75</v>
+      </c>
+      <c r="Y37" t="s">
+        <v>228</v>
+      </c>
       <c r="Z37" s="53">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>99.5</v>
+      </c>
+      <c r="AA37">
+        <v>70</v>
+      </c>
+      <c r="AB37" t="s">
+        <v>119</v>
+      </c>
+      <c r="AC37" t="s">
+        <v>227</v>
       </c>
       <c r="AD37">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AE37">
         <v>0</v>
@@ -5832,15 +5874,33 @@
       </c>
       <c r="AN37">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>9.5</v>
+      </c>
+      <c r="AO37">
+        <v>0</v>
+      </c>
+      <c r="AP37">
+        <v>0</v>
+      </c>
+      <c r="AQ37">
+        <v>0</v>
+      </c>
+      <c r="AR37">
+        <v>2</v>
       </c>
       <c r="AS37">
         <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="AT37">
         <v>0</v>
       </c>
       <c r="AU37">
         <f t="shared" si="4"/>
         <v>0</v>
+      </c>
+      <c r="AV37">
+        <v>9.5</v>
       </c>
     </row>
     <row r="38" spans="3:48" x14ac:dyDescent="0.25">
@@ -5860,14 +5920,20 @@
       <c r="S38" s="49">
         <v>42817</v>
       </c>
-      <c r="T38" s="50"/>
-      <c r="U38" s="51"/>
+      <c r="T38" s="50" t="s">
+        <v>63</v>
+      </c>
+      <c r="U38" s="51" t="s">
+        <v>229</v>
+      </c>
       <c r="V38" s="43">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="W38" s="52"/>
-      <c r="X38" s="52"/>
+      <c r="X38" s="52">
+        <v>0</v>
+      </c>
       <c r="Z38" s="53">
         <f t="shared" si="0"/>
         <v>0</v>

</xml_diff>

<commit_message>
Finanzas de Febreriwi terminadas
</commit_message>
<xml_diff>
--- a/Finanzas/Febrero_2017.xlsx
+++ b/Finanzas/Febrero_2017.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="267">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -799,6 +799,45 @@
   <si>
     <t>Formato</t>
   </si>
+  <si>
+    <t>Pleito Basura</t>
+  </si>
+  <si>
+    <t>Sra Lety</t>
+  </si>
+  <si>
+    <t>Ingles (27-30 mar)</t>
+  </si>
+  <si>
+    <t>Para Copias</t>
+  </si>
+  <si>
+    <t>No Camila</t>
+  </si>
+  <si>
+    <t>Uber Enana</t>
+  </si>
+  <si>
+    <t>Café con Javs</t>
+  </si>
+  <si>
+    <t>Clase Bayes</t>
+  </si>
+  <si>
+    <t>Tortas Filosofía</t>
+  </si>
+  <si>
+    <t>Agua mineral;Twist; Krespy Kreme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maíz </t>
+  </si>
+  <si>
+    <t>Crepas (Jaime)</t>
+  </si>
+  <si>
+    <t>Deposito Papá Uber Enana</t>
+  </si>
 </sst>
 </file>
 
@@ -1126,7 +1165,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1247,7 +1286,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1279,6 +1317,9 @@
     <xf numFmtId="0" fontId="7" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1576,7 +1617,7 @@
   <dimension ref="A1:BE964"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U44" sqref="U44"/>
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1603,7 +1644,7 @@
       <c r="C1" s="56">
         <v>42782</v>
       </c>
-      <c r="D1" s="82" t="s">
+      <c r="D1" s="81" t="s">
         <v>146</v>
       </c>
       <c r="P1" s="78"/>
@@ -1648,9 +1689,9 @@
       <c r="C2" s="58">
         <v>9702</v>
       </c>
-      <c r="D2" s="86">
+      <c r="D2" s="85">
         <f>L3-C2</f>
-        <v>-4788.6499999999996</v>
+        <v>-5184.9299999999994</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>2</v>
@@ -1777,7 +1818,7 @@
       </c>
       <c r="L3" s="27">
         <f>(SUM(C2,(E11:E501),(K11:K500)))-(SUM((D11:D501),(C11:C501)))</f>
-        <v>4913.3500000000004</v>
+        <v>4517.0700000000006</v>
       </c>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
@@ -1892,9 +1933,9 @@
       <c r="M4" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="N4" s="101">
+      <c r="N4" s="100">
         <f>L3+L9</f>
-        <v>29082.35</v>
+        <v>28686.07</v>
       </c>
       <c r="S4" s="49">
         <v>42783</v>
@@ -1992,7 +2033,7 @@
       </c>
       <c r="AZ4" s="64">
         <f>(SUM((AO3:AO520)))-(SUM((AS3:AS520)))</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="BA4" s="64"/>
     </row>
@@ -2118,7 +2159,7 @@
       </c>
       <c r="L6" s="54">
         <f>(SUM((Q11:Q501),(V3:V520)))-(SUM(E11:E501))</f>
-        <v>155.5</v>
+        <v>-153</v>
       </c>
       <c r="M6" s="32"/>
       <c r="N6" s="32"/>
@@ -3057,7 +3098,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AT13" s="81">
+      <c r="AT13" s="80">
         <v>0</v>
       </c>
       <c r="AU13">
@@ -3208,11 +3249,11 @@
         <v>120</v>
       </c>
       <c r="C15" s="13"/>
-      <c r="D15" s="80">
+      <c r="D15" s="101">
         <v>165.23</v>
       </c>
       <c r="E15" s="14"/>
-      <c r="F15" s="92" t="s">
+      <c r="F15" s="91" t="s">
         <v>244</v>
       </c>
       <c r="G15" s="59"/>
@@ -3348,7 +3389,7 @@
         <v>132</v>
       </c>
       <c r="C16" s="13"/>
-      <c r="D16" s="80">
+      <c r="D16" s="101">
         <v>169.93</v>
       </c>
       <c r="E16" s="14"/>
@@ -3403,7 +3444,7 @@
       <c r="Y16" t="s">
         <v>156</v>
       </c>
-      <c r="Z16" s="84">
+      <c r="Z16" s="83">
         <f t="shared" si="0"/>
         <v>125.5</v>
       </c>
@@ -3507,9 +3548,15 @@
         <f t="shared" si="5"/>
         <v>100</v>
       </c>
-      <c r="N17" s="59"/>
-      <c r="O17" s="59"/>
-      <c r="P17" s="59"/>
+      <c r="N17" s="60">
+        <v>42824</v>
+      </c>
+      <c r="O17" s="59" t="s">
+        <v>255</v>
+      </c>
+      <c r="P17" s="59" t="s">
+        <v>256</v>
+      </c>
       <c r="Q17" s="39"/>
       <c r="S17" s="49">
         <v>42796</v>
@@ -3647,7 +3694,7 @@
       <c r="U18" s="51" t="s">
         <v>164</v>
       </c>
-      <c r="V18" s="85">
+      <c r="V18" s="84">
         <f t="shared" si="3"/>
         <v>-15.5</v>
       </c>
@@ -3994,7 +4041,7 @@
       <c r="B21" t="s">
         <v>150</v>
       </c>
-      <c r="C21" s="87"/>
+      <c r="C21" s="86"/>
       <c r="D21" s="12">
         <v>17.22</v>
       </c>
@@ -4159,7 +4206,7 @@
       <c r="W22" s="52">
         <v>75</v>
       </c>
-      <c r="X22" s="88"/>
+      <c r="X22" s="87"/>
       <c r="Z22" s="53">
         <f t="shared" si="0"/>
         <v>60.5</v>
@@ -4492,11 +4539,11 @@
         <v>188</v>
       </c>
       <c r="C25" s="13"/>
-      <c r="D25" s="93">
+      <c r="D25" s="92">
         <v>142.35</v>
       </c>
       <c r="E25" s="14"/>
-      <c r="G25" s="89" t="s">
+      <c r="G25" s="88" t="s">
         <v>30</v>
       </c>
       <c r="H25" s="59" t="s">
@@ -4553,7 +4600,7 @@
       <c r="AD25">
         <v>10</v>
       </c>
-      <c r="AE25" s="91">
+      <c r="AE25" s="90">
         <v>12</v>
       </c>
       <c r="AF25">
@@ -4690,7 +4737,7 @@
       <c r="AF26">
         <v>100</v>
       </c>
-      <c r="AG26" s="91">
+      <c r="AG26" s="90">
         <v>20</v>
       </c>
       <c r="AH26">
@@ -5010,7 +5057,7 @@
       <c r="H29" s="59" t="s">
         <v>153</v>
       </c>
-      <c r="I29" s="83" t="s">
+      <c r="I29" s="82" t="s">
         <v>154</v>
       </c>
       <c r="J29" s="24">
@@ -5133,22 +5180,22 @@
         <v>201</v>
       </c>
       <c r="E30" s="14"/>
-      <c r="G30" s="60">
+      <c r="G30" s="96">
         <v>42795</v>
       </c>
-      <c r="H30" s="59" t="s">
+      <c r="H30" s="64" t="s">
         <v>158</v>
       </c>
-      <c r="I30" s="59" t="s">
+      <c r="I30" s="64" t="s">
         <v>159</v>
       </c>
-      <c r="J30" s="24">
+      <c r="J30" s="97">
         <v>20</v>
       </c>
-      <c r="K30" s="75" t="s">
+      <c r="K30" s="102" t="s">
         <v>184</v>
       </c>
-      <c r="L30" s="21">
+      <c r="L30" s="99">
         <v>0</v>
       </c>
       <c r="N30" s="59"/>
@@ -5164,7 +5211,7 @@
       <c r="U30" s="51" t="s">
         <v>208</v>
       </c>
-      <c r="V30" s="85">
+      <c r="V30" s="84">
         <f t="shared" si="3"/>
         <v>-25.5</v>
       </c>
@@ -5247,7 +5294,7 @@
       </c>
     </row>
     <row r="31" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A31" s="90">
+      <c r="A31" s="89">
         <v>42805</v>
       </c>
       <c r="B31" t="s">
@@ -5258,7 +5305,7 @@
         <v>52.79</v>
       </c>
       <c r="E31" s="14"/>
-      <c r="G31" s="97">
+      <c r="G31" s="96">
         <v>42816</v>
       </c>
       <c r="H31" s="64" t="s">
@@ -5267,13 +5314,13 @@
       <c r="I31" s="64" t="s">
         <v>217</v>
       </c>
-      <c r="J31" s="98">
+      <c r="J31" s="97">
         <v>150</v>
       </c>
-      <c r="K31" s="99" t="s">
+      <c r="K31" s="98" t="s">
         <v>246</v>
       </c>
-      <c r="L31" s="100">
+      <c r="L31" s="99">
         <v>0</v>
       </c>
       <c r="N31" s="59"/>
@@ -5313,7 +5360,7 @@
       <c r="AD31">
         <v>60</v>
       </c>
-      <c r="AE31" s="91">
+      <c r="AE31" s="90">
         <v>128</v>
       </c>
       <c r="AF31">
@@ -5344,7 +5391,7 @@
         <f t="shared" si="6"/>
         <v>34.5</v>
       </c>
-      <c r="AO31" s="91">
+      <c r="AO31" s="90">
         <v>20</v>
       </c>
       <c r="AP31">
@@ -5492,7 +5539,7 @@
         <v>30.5</v>
       </c>
     </row>
-    <row r="33" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A33" s="34">
         <v>42812</v>
       </c>
@@ -5546,7 +5593,7 @@
         <f t="shared" si="0"/>
         <v>94</v>
       </c>
-      <c r="AA33" s="91">
+      <c r="AA33" s="90">
         <v>62</v>
       </c>
       <c r="AB33" t="s">
@@ -5616,7 +5663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A34" s="34">
         <v>42821</v>
       </c>
@@ -5726,18 +5773,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A35" s="96">
+    <row r="35" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A35" s="95">
         <v>42821</v>
       </c>
-      <c r="B35" s="94" t="s">
+      <c r="B35" s="93" t="s">
         <v>245</v>
       </c>
-      <c r="C35" s="94"/>
-      <c r="D35" s="94">
+      <c r="C35" s="93"/>
+      <c r="D35" s="93">
         <v>-642</v>
       </c>
-      <c r="E35" s="95"/>
+      <c r="E35" s="94"/>
       <c r="G35" s="59"/>
       <c r="H35" s="59"/>
       <c r="I35" s="59"/>
@@ -5839,9 +5886,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A36" s="34">
+        <v>42823</v>
+      </c>
       <c r="C36" s="13"/>
-      <c r="D36" s="12"/>
+      <c r="D36" s="12">
+        <v>156.22</v>
+      </c>
       <c r="E36" s="14"/>
       <c r="G36" s="59"/>
       <c r="H36" s="59"/>
@@ -5946,9 +5998,17 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="37" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A37" s="34">
+        <v>42823</v>
+      </c>
+      <c r="B37" t="s">
+        <v>259</v>
+      </c>
       <c r="C37" s="13"/>
-      <c r="D37" s="12"/>
+      <c r="D37" s="12">
+        <v>219.16</v>
+      </c>
       <c r="E37" s="14"/>
       <c r="G37" s="59"/>
       <c r="H37" s="59"/>
@@ -6056,9 +6116,17 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="38" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="C38" s="13"/>
-      <c r="D38" s="12"/>
+    <row r="38" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A38" s="34">
+        <v>42824</v>
+      </c>
+      <c r="B38" t="s">
+        <v>260</v>
+      </c>
+      <c r="C38" s="86"/>
+      <c r="D38" s="12">
+        <v>53</v>
+      </c>
       <c r="E38" s="14"/>
       <c r="G38" s="59"/>
       <c r="H38" s="59"/>
@@ -6166,9 +6234,17 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A39" s="34">
+        <v>42825</v>
+      </c>
+      <c r="B39" t="s">
+        <v>194</v>
+      </c>
       <c r="C39" s="13"/>
-      <c r="D39" s="12"/>
+      <c r="D39" s="12">
+        <v>217.9</v>
+      </c>
       <c r="E39" s="14"/>
       <c r="G39" s="59"/>
       <c r="H39" s="59"/>
@@ -6276,10 +6352,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A40" s="34">
+        <v>42825</v>
+      </c>
+      <c r="B40" t="s">
+        <v>266</v>
+      </c>
       <c r="C40" s="13"/>
       <c r="D40" s="12"/>
-      <c r="E40" s="14"/>
+      <c r="E40" s="14">
+        <v>250</v>
+      </c>
       <c r="G40" s="59"/>
       <c r="H40" s="59"/>
       <c r="I40" s="59"/>
@@ -6381,7 +6465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:49" x14ac:dyDescent="0.25">
       <c r="C41" s="13"/>
       <c r="D41" s="12"/>
       <c r="E41" s="14"/>
@@ -6485,7 +6569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:49" x14ac:dyDescent="0.25">
       <c r="C42" s="13"/>
       <c r="D42" s="12"/>
       <c r="E42" s="14"/>
@@ -6584,7 +6668,7 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="43" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:49" x14ac:dyDescent="0.25">
       <c r="C43" s="13"/>
       <c r="D43" s="12"/>
       <c r="E43" s="14"/>
@@ -6609,7 +6693,7 @@
       </c>
       <c r="V43" s="43">
         <f t="shared" si="3"/>
-        <v>-29</v>
+        <v>-38.5</v>
       </c>
       <c r="W43" s="52">
         <v>75</v>
@@ -6617,7 +6701,7 @@
       <c r="X43" s="52"/>
       <c r="Z43" s="53">
         <f t="shared" si="0"/>
-        <v>104</v>
+        <v>113.5</v>
       </c>
       <c r="AA43">
         <v>60</v>
@@ -6660,7 +6744,7 @@
       </c>
       <c r="AN43">
         <f t="shared" si="6"/>
-        <v>25</v>
+        <v>34.5</v>
       </c>
       <c r="AO43">
         <v>20</v>
@@ -6686,10 +6770,10 @@
         <v>0</v>
       </c>
       <c r="AV43">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="44" spans="1:48" x14ac:dyDescent="0.25">
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:49" x14ac:dyDescent="0.25">
       <c r="C44" s="13"/>
       <c r="D44" s="12"/>
       <c r="E44" s="14"/>
@@ -6709,19 +6793,37 @@
       <c r="T44" s="50" t="s">
         <v>248</v>
       </c>
-      <c r="U44" s="51"/>
+      <c r="U44" s="51" t="s">
+        <v>254</v>
+      </c>
       <c r="V44" s="43">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="W44" s="52"/>
-      <c r="X44" s="52"/>
+        <v>-21.5</v>
+      </c>
+      <c r="W44" s="52">
+        <v>80</v>
+      </c>
+      <c r="X44" s="52">
+        <v>10</v>
+      </c>
+      <c r="Y44" t="s">
+        <v>257</v>
+      </c>
       <c r="Z44" s="53">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>111.5</v>
+      </c>
+      <c r="AA44">
+        <v>69</v>
+      </c>
+      <c r="AB44" t="s">
+        <v>185</v>
+      </c>
+      <c r="AC44" t="s">
+        <v>219</v>
       </c>
       <c r="AD44">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AE44">
         <v>0</v>
@@ -6752,18 +6854,36 @@
       </c>
       <c r="AN44">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>35.5</v>
+      </c>
+      <c r="AO44" s="12">
+        <v>20</v>
+      </c>
+      <c r="AP44">
+        <v>2</v>
+      </c>
+      <c r="AQ44">
+        <v>0</v>
+      </c>
+      <c r="AR44">
+        <v>2</v>
       </c>
       <c r="AS44">
         <f t="shared" si="7"/>
+        <v>22</v>
+      </c>
+      <c r="AT44">
         <v>0</v>
       </c>
       <c r="AU44">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AV44">
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:49" x14ac:dyDescent="0.25">
       <c r="C45" s="13"/>
       <c r="D45" s="12"/>
       <c r="E45" s="14"/>
@@ -6783,25 +6903,38 @@
       <c r="T45" s="50" t="s">
         <v>63</v>
       </c>
-      <c r="U45" s="74"/>
+      <c r="U45" s="103" t="s">
+        <v>258</v>
+      </c>
       <c r="V45" s="43">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="W45" s="52"/>
+        <v>-112.5</v>
+      </c>
+      <c r="W45" s="52">
+        <v>75</v>
+      </c>
       <c r="X45" s="52"/>
       <c r="Z45" s="53">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>187.5</v>
+      </c>
+      <c r="AA45">
+        <v>95</v>
+      </c>
+      <c r="AB45" s="78" t="s">
+        <v>262</v>
+      </c>
+      <c r="AC45" t="s">
+        <v>263</v>
       </c>
       <c r="AD45">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="AE45">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AF45">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="AG45">
         <v>0</v>
@@ -6826,18 +6959,36 @@
       </c>
       <c r="AN45">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>26.5</v>
+      </c>
+      <c r="AO45" s="12">
+        <v>12</v>
+      </c>
+      <c r="AP45" s="12">
+        <v>1</v>
+      </c>
+      <c r="AQ45">
+        <v>0</v>
+      </c>
+      <c r="AR45">
+        <v>2</v>
       </c>
       <c r="AS45">
         <f t="shared" si="7"/>
+        <v>16</v>
+      </c>
+      <c r="AT45">
         <v>0</v>
       </c>
       <c r="AU45">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AV45">
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:49" x14ac:dyDescent="0.25">
       <c r="C46" s="13"/>
       <c r="D46" s="12"/>
       <c r="E46" s="14"/>
@@ -6857,19 +7008,34 @@
       <c r="T46" s="50" t="s">
         <v>83</v>
       </c>
-      <c r="U46" s="51"/>
+      <c r="U46" s="51" t="s">
+        <v>261</v>
+      </c>
       <c r="V46" s="43">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="W46" s="52"/>
-      <c r="X46" s="52"/>
+        <v>85</v>
+      </c>
+      <c r="W46" s="52">
+        <v>75</v>
+      </c>
+      <c r="X46" s="52">
+        <v>20</v>
+      </c>
       <c r="Z46" s="53">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="AA46">
+        <v>0</v>
+      </c>
+      <c r="AB46" s="78" t="s">
+        <v>265</v>
+      </c>
+      <c r="AC46" t="s">
+        <v>264</v>
       </c>
       <c r="AD46">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AE46">
         <v>0</v>
@@ -6910,8 +7076,9 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AW46" s="40"/>
+    </row>
+    <row r="47" spans="1:49" x14ac:dyDescent="0.25">
       <c r="C47" s="13"/>
       <c r="D47" s="12"/>
       <c r="E47" s="14"/>
@@ -6981,7 +7148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:49" x14ac:dyDescent="0.25">
       <c r="C48" s="13"/>
       <c r="D48" s="12"/>
       <c r="E48" s="14"/>

</xml_diff>